<commit_message>
Updating testHelpers module. Adding xls (excel) DataProviderLoader.
</commit_message>
<xml_diff>
--- a/testHelpers/src/main/resources/testData/testData.xlsx
+++ b/testHelpers/src/main/resources/testData/testData.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Projects\document-archive\testHelpers\src\main\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A01B1FD4-B057-499C-A98D-67B3A0A40DC3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7FBE631-62A3-4E61-95D0-E773B49D752E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="usersList" sheetId="1" r:id="rId1"/>
-    <sheet name="documentsList" sheetId="2" r:id="rId2"/>
+    <sheet name="rolesList" sheetId="3" r:id="rId1"/>
+    <sheet name="usersList" sheetId="1" r:id="rId2"/>
+    <sheet name="documentsList" sheetId="2" r:id="rId3"/>
+    <sheet name="documentMetaDataList" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="42">
   <si>
     <t>ROLE</t>
   </si>
@@ -100,16 +102,58 @@
     <t>PATH_TO_DOCUMENT</t>
   </si>
   <si>
-    <t>/documentsList/documents/testDocumentMariusz1.docx</t>
-  </si>
-  <si>
-    <t>/documentsList/documents/testDocumentMariusz2.docx</t>
-  </si>
-  <si>
-    <t>/documentsList/documents/testDocumentUser123.docx</t>
-  </si>
-  <si>
-    <t>/documentsList/documents/testDocumentUser1234.pdf</t>
+    <t>ROLE_NAME</t>
+  </si>
+  <si>
+    <t>ADMIN</t>
+  </si>
+  <si>
+    <t>DOCUMENT_NAME</t>
+  </si>
+  <si>
+    <t>META_DATA_NAME</t>
+  </si>
+  <si>
+    <t>META_DATA_VALUE</t>
+  </si>
+  <si>
+    <t>testDocumentMariusz1.docx</t>
+  </si>
+  <si>
+    <t>metaDataName1</t>
+  </si>
+  <si>
+    <t>metaDataValue1</t>
+  </si>
+  <si>
+    <t>metaDataName2</t>
+  </si>
+  <si>
+    <t>metaDataValue2</t>
+  </si>
+  <si>
+    <t>metaDataName3</t>
+  </si>
+  <si>
+    <t>metaDataValue3</t>
+  </si>
+  <si>
+    <t>metaDataName4</t>
+  </si>
+  <si>
+    <t>metaDataValue4</t>
+  </si>
+  <si>
+    <t>testData/documents/testDocumentMariusz1.docx</t>
+  </si>
+  <si>
+    <t>testData/documents/testDocumentMariusz2.docx</t>
+  </si>
+  <si>
+    <t>testData/documents/testDocumentUser123.docx</t>
+  </si>
+  <si>
+    <t>testData/documents/testDocumentUser1234.pdf</t>
   </si>
 </sst>
 </file>
@@ -426,6 +470,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47825D57-C3C5-4DF0-A346-30856FEF6D54}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L28" sqref="L28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
@@ -528,18 +605,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{546CD878-BAB3-4C23-8D74-002783B4A037}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="52.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -555,7 +632,7 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -563,7 +640,7 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -571,7 +648,7 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -579,7 +656,98 @@
         <v>18</v>
       </c>
       <c r="B5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D8C661A-1589-4605-8BEA-8297A91D8062}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
         <v>27</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>